<commit_message>
Added Decision Tree Solution
</commit_message>
<xml_diff>
--- a/4. Tree Based Algorithms/Decision Tree Example.xlsx
+++ b/4. Tree Based Algorithms/Decision Tree Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paragpradhan/Documents/Data Science Course/DSB2/4. Tree Based Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A509B8B-DFD9-344B-8EA4-51E184969E1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D196C3C4-04F6-C44C-9EC2-C842F067A276}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16220" xr2:uid="{E5244438-C132-7043-BC96-08C69C5D2FC1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E5244438-C132-7043-BC96-08C69C5D2FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
   <si>
     <t>Outlook</t>
   </si>
@@ -136,15 +136,6 @@
     <t>Gain(Outlook = Overcast) = </t>
   </si>
   <si>
-    <t>Entropy (Decision | Windy = False)</t>
-  </si>
-  <si>
-    <t>Entropy (Decision | Windy = True)</t>
-  </si>
-  <si>
-    <t>Gain(Decision | Windy)</t>
-  </si>
-  <si>
     <t>Gain(Outlook = rainy | Humidity)</t>
   </si>
   <si>
@@ -161,13 +152,34 @@
   </si>
   <si>
     <t>Gain(Outlook = sunny | Humidity)</t>
+  </si>
+  <si>
+    <t>Entropy (Outlook = sunny | Windy =False)</t>
+  </si>
+  <si>
+    <t>Entropy (outlook = sunny | Windy = True)</t>
+  </si>
+  <si>
+    <t>Gain(Outlook = sunny | Windy)</t>
+  </si>
+  <si>
+    <t>** No need to split</t>
+  </si>
+  <si>
+    <t>Gain(Outlook = rainy | Windy)</t>
+  </si>
+  <si>
+    <t>Entropy (Outlook = rainy | Windy = False)</t>
+  </si>
+  <si>
+    <t>Entropy (Outlook = rainy | Windy = True)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -560,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904E8A30-2D21-7F4A-A6FC-205D3F0C16A8}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="3" bestFit="1" customWidth="1"/>
@@ -577,7 +589,7 @@
     <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -611,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -631,7 +643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -651,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -672,7 +684,7 @@
         <v>0.94028595867063092</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -686,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -706,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -726,7 +738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -746,7 +758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -760,7 +772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -780,7 +792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -794,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
@@ -812,7 +824,7 @@
         <v>0.81127812445913283</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -832,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -850,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F17" s="8" t="s">
         <v>18</v>
       </c>
@@ -859,7 +871,7 @@
         <v>4.8127030408269322E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19" s="4" t="s">
         <v>25</v>
       </c>
@@ -868,7 +880,7 @@
         <v>0.98522813603425163</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
         <v>26</v>
       </c>
@@ -877,7 +889,7 @@
         <v>0.59167277858232747</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21" s="8" t="s">
         <v>27</v>
       </c>
@@ -886,7 +898,7 @@
         <v>0.15183550136234136</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23" s="4" t="s">
         <v>28</v>
       </c>
@@ -898,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="4" t="s">
         <v>29</v>
       </c>
@@ -907,7 +919,7 @@
         <v>0.97095059445466858</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" s="4" t="s">
         <v>30</v>
       </c>
@@ -916,7 +928,7 @@
         <v>0.97095059445466858</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F26" s="8" t="s">
         <v>31</v>
       </c>
@@ -925,7 +937,7 @@
         <v>0.24674981977443911</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,7 +951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>3</v>
       </c>
@@ -956,8 +968,11 @@
         <v>32</v>
       </c>
       <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
@@ -971,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>3</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,10 +1028,14 @@
         <v>11</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="G38" s="3">
+        <f>-(1/2)*LOG(1/2,2)-(1/2)*LOG(1/2,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>7</v>
       </c>
@@ -1030,10 +1049,14 @@
         <v>5</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>34</v>
+      </c>
+      <c r="G39" s="3">
+        <f>-(1/3)*LOG(1/3,2)-(2/3)*LOG(2/3,2)</f>
+        <v>0.91829583405448956</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
@@ -1047,11 +1070,14 @@
         <v>5</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7">
+        <v>33</v>
+      </c>
+      <c r="G40" s="7">
+        <f>G24 - (2/5)*G38 - (3/5)*G39</f>
+        <v>1.9973094021974891E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>7</v>
       </c>
@@ -1079,10 +1105,13 @@
         <v>5</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
@@ -1096,16 +1125,22 @@
         <v>8</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>45</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F44" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="47" spans="1:7">
+        <v>43</v>
+      </c>
+      <c r="G44" s="7">
+        <f>G24-(3/5)*G42 - (2/5)*G43</f>
+        <v>0.97095059445466858</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,10 +1154,13 @@
         <v>11</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>36</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>9</v>
       </c>
@@ -1136,10 +1174,13 @@
         <v>8</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>37</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>9</v>
       </c>
@@ -1153,11 +1194,14 @@
         <v>8</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="1:7">
+        <v>38</v>
+      </c>
+      <c r="G49" s="3">
+        <f>G25-(3/5)*G47-(2/5)*G48</f>
+        <v>0.97095059445466858</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -1184,8 +1228,15 @@
       <c r="D51" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="F51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G51" s="3">
+        <f xml:space="preserve"> -(2/3)*LOG(2/3,2)-(1/3)*LOG(1/3,2)</f>
+        <v>0.91829583405448956</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>9</v>
       </c>
@@ -1197,6 +1248,21 @@
       </c>
       <c r="D52" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F53" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G53" s="7">
+        <f>G25-(3/5)*G51-(2/5)*G52</f>
+        <v>1.9973094021974891E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>